<commit_message>
Update OPIS and Supplier prompts with examples, and mappings with new entries for OPIS and Luke Oil
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="158">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -87,15 +87,30 @@
     <t xml:space="preserve">MPC</t>
   </si>
   <si>
+    <t xml:space="preserve">Hartford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Streett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunoco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExxonMobil</t>
+  </si>
+  <si>
     <t xml:space="preserve">ULSD</t>
   </si>
   <si>
     <t xml:space="preserve">#2ULSD</t>
   </si>
   <si>
-    <t xml:space="preserve">87E10 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Reg 87E10</t>
   </si>
   <si>
@@ -234,12 +249,87 @@
     <t xml:space="preserve">CFP #2 ULSD</t>
   </si>
   <si>
+    <t xml:space="preserve">Unl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid 89E10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre 91E10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULS No.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULS2 RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULS2 WNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULS2D WNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre 93E10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conv 87E10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B11 WB CLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B11W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B11 WB DYE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B11WD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B17 WB CLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B17W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B17 WB DYE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B17WD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Pure Ethanol w/out RINS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethanol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross E-75 Unl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross E-85 Unl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-85</t>
+  </si>
+  <si>
     <t xml:space="preserve">Condition</t>
   </si>
   <si>
-    <t xml:space="preserve">Hartford</t>
-  </si>
-  <si>
     <t xml:space="preserve">PH-PH-HARTFORD</t>
   </si>
   <si>
@@ -397,15 +487,25 @@
   </si>
   <si>
     <t xml:space="preserve">Wallis Heyworth MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WOODRIVER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAHOKIA-IL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARTFORD-IL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -488,7 +588,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -501,12 +601,8 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -517,7 +613,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -525,7 +621,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -721,10 +817,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -742,42 +838,42 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -785,7 +881,7 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -817,7 +913,7 @@
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -825,7 +921,7 @@
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -873,8 +969,48 @@
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -893,352 +1029,504 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="18.26"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>23</v>
+      <c r="A3" s="6" t="n">
+        <v>870000000000</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="n">
+        <v>930000000000</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1257,303 +1545,331 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="18.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="5" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="10.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="4" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>70</v>
+      <c r="C1" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="A3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>79</v>
+      <c r="A4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="9"/>
+      <c r="A6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="9"/>
+      <c r="A7" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="9"/>
+      <c r="A8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="9"/>
+      <c r="A9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="9"/>
+      <c r="A10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="9"/>
+      <c r="A11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="9"/>
+      <c r="A12" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="9"/>
+      <c r="A13" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" s="9"/>
+      <c r="A14" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="9"/>
+      <c r="A15" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="9"/>
+      <c r="A16" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="9"/>
+      <c r="A17" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="9"/>
+      <c r="A18" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="9"/>
+      <c r="A19" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C31" s="9"/>
+      <c r="C34" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update mappings.xlsx to cleaned version (manual domain fix)
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Luke Oil</t>
   </si>
   <si>
-    <t xml:space="preserve">lukebrands.com </t>
+    <t xml:space="preserve">lukebrands.com</t>
   </si>
   <si>
     <t xml:space="preserve">Wallis Oil Company</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Wallis Oil</t>
   </si>
   <si>
-    <t xml:space="preserve">wallisco.com </t>
+    <t xml:space="preserve">wallisco.com</t>
   </si>
   <si>
     <t xml:space="preserve">By-Lo Oil Company  </t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">By-Lo Oil</t>
   </si>
   <si>
-    <t xml:space="preserve">bylooil.com </t>
+    <t xml:space="preserve">bylooil.com</t>
   </si>
   <si>
     <t xml:space="preserve">World Kinect          </t>
@@ -67,13 +67,13 @@
     <t xml:space="preserve">World Kinect</t>
   </si>
   <si>
-    <t xml:space="preserve">world-kinect.com </t>
+    <t xml:space="preserve">world-kinect.com</t>
   </si>
   <si>
     <t xml:space="preserve">OPIS</t>
   </si>
   <si>
-    <t xml:space="preserve">opisnet.com </t>
+    <t xml:space="preserve">opisnet.com</t>
   </si>
   <si>
     <t xml:space="preserve">FleetFuelsNW</t>
@@ -538,7 +538,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,12 +568,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -625,7 +619,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -634,7 +628,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -642,7 +636,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -650,19 +644,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -670,20 +652,8 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -884,8 +854,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,29 +894,29 @@
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -957,7 +927,7 @@
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -998,7 +968,7 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1009,162 +979,162 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1193,15 +1163,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.26"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1214,7 +1184,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="8" t="n">
         <v>870000000000</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1598,7 +1568,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="13" t="n">
+      <c r="A51" s="8" t="n">
         <v>930000000000</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -1709,20 +1679,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="10.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="12" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1733,7 +1703,7 @@
       <c r="B2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -1742,7 +1712,7 @@
       <c r="B3" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -1773,7 +1743,7 @@
       <c r="B6" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -1782,7 +1752,7 @@
       <c r="B7" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
@@ -1791,7 +1761,7 @@
       <c r="B8" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
@@ -1800,7 +1770,7 @@
       <c r="B9" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
@@ -1809,7 +1779,7 @@
       <c r="B10" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
@@ -1818,7 +1788,7 @@
       <c r="B11" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
@@ -1827,7 +1797,7 @@
       <c r="B12" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
@@ -1836,7 +1806,7 @@
       <c r="B13" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -1845,7 +1815,7 @@
       <c r="B14" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
@@ -1854,7 +1824,7 @@
       <c r="B15" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
@@ -1863,7 +1833,7 @@
       <c r="B16" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
@@ -1872,7 +1842,7 @@
       <c r="B17" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
@@ -1881,7 +1851,7 @@
       <c r="B18" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
@@ -1890,7 +1860,7 @@
       <c r="B19" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
@@ -1899,7 +1869,7 @@
       <c r="B20" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
@@ -1908,7 +1878,7 @@
       <c r="B21" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
@@ -1917,7 +1887,7 @@
       <c r="B22" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
@@ -1926,7 +1896,7 @@
       <c r="B23" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
@@ -1935,7 +1905,7 @@
       <c r="B24" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
@@ -1944,7 +1914,7 @@
       <c r="B25" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
@@ -1953,7 +1923,7 @@
       <c r="B26" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C26" s="15"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
@@ -1962,7 +1932,7 @@
       <c r="B27" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
@@ -1971,7 +1941,7 @@
       <c r="B28" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
@@ -1980,7 +1950,7 @@
       <c r="B29" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
@@ -1989,7 +1959,7 @@
       <c r="B30" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
@@ -1998,7 +1968,7 @@
       <c r="B31" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
@@ -2007,7 +1977,7 @@
       <c r="B32" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
@@ -2016,7 +1986,7 @@
       <c r="B33" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="15"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">

</xml_diff>

<commit_message>
Update parser.py and mappings.xlsx with Supply prefix extraction logic
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="SupplyMappings" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="ProductMappings" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="TerminalMappings" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="SupplyLookupMappings" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="ProductMappings" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="TerminalMappings" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="212">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -134,6 +135,138 @@
   </si>
   <si>
     <t xml:space="preserve">ExxonMobil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BP-KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FH-MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flint Hills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMK-MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC-HEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marathon Petroleum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDS Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinclair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVR Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIKTRIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WALLIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUSKET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Musket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMK-KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNBRANDED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unbranded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PETRO-CAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petro-Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONOCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conoco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brentwood Oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEMINI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gemini Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIDCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midcoast Energy</t>
   </si>
   <si>
     <t xml:space="preserve">ULSD</t>
@@ -538,7 +671,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +700,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -619,7 +759,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -649,6 +789,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -854,7 +998,7 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1155,6 +1299,290 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1177,482 +1605,482 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="9" t="n">
         <v>870000000000</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>85</v>
+        <v>129</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="n">
+      <c r="A51" s="9" t="n">
         <v>930000000000</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>101</v>
+        <v>145</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>104</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1666,7 +2094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1693,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,299 +2129,299 @@
         <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="9"/>
+        <v>156</v>
+      </c>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="9"/>
+        <v>158</v>
+      </c>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="9"/>
+        <v>165</v>
+      </c>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="9"/>
+        <v>167</v>
+      </c>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>124</v>
+        <v>168</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="9"/>
+        <v>169</v>
+      </c>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="9"/>
+        <v>171</v>
+      </c>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>128</v>
+        <v>172</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="9"/>
+        <v>173</v>
+      </c>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="9"/>
+        <v>160</v>
+      </c>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>131</v>
+        <v>175</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="9"/>
+        <v>176</v>
+      </c>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="9"/>
+        <v>178</v>
+      </c>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>135</v>
+        <v>179</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="9"/>
+        <v>167</v>
+      </c>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="9"/>
+        <v>173</v>
+      </c>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>137</v>
+        <v>181</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C16" s="9"/>
+        <v>173</v>
+      </c>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="9"/>
+        <v>160</v>
+      </c>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="9"/>
+        <v>160</v>
+      </c>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="9"/>
+        <v>188</v>
+      </c>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C22" s="9"/>
+        <v>190</v>
+      </c>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C23" s="9"/>
+        <v>192</v>
+      </c>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="9"/>
+        <v>194</v>
+      </c>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="9"/>
+        <v>196</v>
+      </c>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C26" s="9"/>
+        <v>198</v>
+      </c>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>155</v>
+        <v>199</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="9"/>
+        <v>200</v>
+      </c>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>157</v>
+        <v>201</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="9"/>
+        <v>202</v>
+      </c>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" s="9"/>
+        <v>204</v>
+      </c>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C30" s="9"/>
+        <v>206</v>
+      </c>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="9"/>
+        <v>208</v>
+      </c>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>165</v>
+        <v>209</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" s="9"/>
+        <v>173</v>
+      </c>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>166</v>
+        <v>210</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C33" s="9"/>
+        <v>160</v>
+      </c>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="C34" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add missing supply prefixes to SupplyLookupMappings and improve extract_position_holder logic
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="214">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t xml:space="preserve">Midcoast Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VL-MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMK</t>
   </si>
   <si>
     <t xml:space="preserve">ULSD</t>
@@ -792,7 +798,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1299,16 +1305,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,6 +1571,22 @@
       </c>
       <c r="B32" s="0" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1605,10 +1627,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,383 +1638,383 @@
         <v>870000000000</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2000,87 +2022,87 @@
         <v>930000000000</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2121,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,299 +2151,299 @@
         <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C34" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update parser and supply mapping: cleaned Wallis, improved Supply resolution
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="213">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -146,133 +146,130 @@
     <t xml:space="preserve">BP-KM</t>
   </si>
   <si>
+    <t xml:space="preserve">BRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brentwood Oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONOCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conoco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVR Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FH-MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flint Hills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEMINI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gemini Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMK-KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMK-MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDS Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIDCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midcoast Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marathon Petroleum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUSKET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Musket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PETRO-CAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petro-Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-KM</t>
+  </si>
+  <si>
     <t xml:space="preserve">PH-PH</t>
   </si>
   <si>
-    <t xml:space="preserve">FH-MG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flint Hills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMK-MG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Growmark</t>
+    <t xml:space="preserve">PHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIKTRIP</t>
   </si>
   <si>
     <t xml:space="preserve">SC-HEP</t>
   </si>
   <si>
-    <t xml:space="preserve">Marathon Petroleum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JDS Energy</t>
+    <t xml:space="preserve">SHELL</t>
   </si>
   <si>
     <t xml:space="preserve">Sinclair</t>
   </si>
   <si>
-    <t xml:space="preserve">CVR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CVR Energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUIKTRIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHELL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WALLIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUSKET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH-KM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMK-KM</t>
-  </si>
-  <si>
     <t xml:space="preserve">UNBRANDED</t>
   </si>
   <si>
     <t xml:space="preserve">Unbranded</t>
   </si>
   <si>
-    <t xml:space="preserve">CHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSX</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALERO</t>
   </si>
   <si>
     <t xml:space="preserve">Valero</t>
   </si>
   <si>
-    <t xml:space="preserve">PH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PETRO-CAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petro-Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONOCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conoco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CENEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brentwood Oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEMINI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gemini Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIDCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midcoast Energy</t>
-  </si>
-  <si>
     <t xml:space="preserve">VL-MG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMK</t>
   </si>
   <si>
     <t xml:space="preserve">ULSD</t>
@@ -1308,7 +1305,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1338,15 +1335,15 @@
         <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,132 +1351,132 @@
         <v>43</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>20</v>
@@ -1487,7 +1484,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>20</v>
@@ -1495,15 +1492,15 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>20</v>
@@ -1511,7 +1508,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>20</v>
@@ -1519,7 +1516,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>20</v>
@@ -1527,31 +1524,31 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>76</v>
@@ -1578,15 +1575,15 @@
         <v>81</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1627,10 +1624,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,383 +1635,383 @@
         <v>870000000000</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2022,87 +2019,87 @@
         <v>930000000000</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2143,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,299 +2148,299 @@
         <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="C3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="C9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>175</v>
       </c>
       <c r="C10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="C12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="C19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="C21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="C22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="C23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="C24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="C25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="C26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="C27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="C28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="C29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>208</v>
       </c>
       <c r="C30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="C31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C34" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update mappings.xlsx with new SupplyLookup entries
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="217">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -269,7 +269,19 @@
     <t xml:space="preserve">Valero</t>
   </si>
   <si>
+    <t xml:space="preserve">VALERO-MG </t>
+  </si>
+  <si>
     <t xml:space="preserve">VL-MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDS/STL/JDS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDS Energy </t>
   </si>
   <si>
     <t xml:space="preserve">ULSD</t>
@@ -762,7 +774,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -797,6 +809,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1302,10 +1318,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1323,267 +1339,291 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1624,482 +1664,482 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="10" t="n">
         <v>870000000000</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="n">
+      <c r="A51" s="10" t="n">
         <v>930000000000</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2140,7 +2180,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,299 +2188,299 @@
         <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="10"/>
+        <v>161</v>
+      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" s="10"/>
+        <v>163</v>
+      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="10"/>
+        <v>170</v>
+      </c>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="10"/>
+        <v>172</v>
+      </c>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C8" s="10"/>
+        <v>174</v>
+      </c>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C9" s="10"/>
+        <v>176</v>
+      </c>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>178</v>
+      </c>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="10"/>
+        <v>165</v>
+      </c>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="10"/>
+        <v>181</v>
+      </c>
+      <c r="C12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>183</v>
+      </c>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14" s="10"/>
+        <v>172</v>
+      </c>
+      <c r="C14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C15" s="10"/>
+        <v>178</v>
+      </c>
+      <c r="C15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C16" s="10"/>
+        <v>178</v>
+      </c>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C17" s="10"/>
+        <v>165</v>
+      </c>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>165</v>
+      </c>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C20" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="C20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>193</v>
+      </c>
+      <c r="C21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C22" s="10"/>
+        <v>195</v>
+      </c>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C23" s="10"/>
+        <v>197</v>
+      </c>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C24" s="10"/>
+        <v>199</v>
+      </c>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C25" s="10"/>
+        <v>201</v>
+      </c>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C26" s="10"/>
+        <v>203</v>
+      </c>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C27" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C28" s="10"/>
+        <v>207</v>
+      </c>
+      <c r="C28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C29" s="10"/>
+        <v>209</v>
+      </c>
+      <c r="C29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C30" s="10"/>
+        <v>211</v>
+      </c>
+      <c r="C30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C31" s="10"/>
+        <v>213</v>
+      </c>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C32" s="10"/>
+        <v>178</v>
+      </c>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C33" s="10"/>
+        <v>165</v>
+      </c>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C34" s="1"/>
     </row>

</xml_diff>

<commit_message>
🐛 Fix SupplyLookupMappings parsing logic to load non-null trimmed rows
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -137,10 +137,10 @@
     <t xml:space="preserve">ExxonMobil</t>
   </si>
   <si>
-    <t xml:space="preserve">prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supply</t>
+    <t xml:space="preserve">Prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supply</t>
   </si>
   <si>
     <t xml:space="preserve">BP-KM</t>
@@ -774,7 +774,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -809,10 +809,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1321,7 +1317,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1611,18 +1607,18 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1671,7 +1667,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="9" t="n">
         <v>870000000000</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2055,7 +2051,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="n">
+      <c r="A51" s="9" t="n">
         <v>930000000000</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -2190,7 +2186,7 @@
       <c r="B2" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -2199,7 +2195,7 @@
       <c r="B3" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -2230,7 +2226,7 @@
       <c r="B6" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -2239,7 +2235,7 @@
       <c r="B7" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
@@ -2248,7 +2244,7 @@
       <c r="B8" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
@@ -2257,7 +2253,7 @@
       <c r="B9" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
@@ -2266,7 +2262,7 @@
       <c r="B10" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
@@ -2275,7 +2271,7 @@
       <c r="B11" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
@@ -2284,7 +2280,7 @@
       <c r="B12" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
@@ -2293,7 +2289,7 @@
       <c r="B13" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -2302,7 +2298,7 @@
       <c r="B14" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
@@ -2311,7 +2307,7 @@
       <c r="B15" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
@@ -2320,7 +2316,7 @@
       <c r="B16" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
@@ -2329,7 +2325,7 @@
       <c r="B17" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
@@ -2338,7 +2334,7 @@
       <c r="B18" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
@@ -2347,7 +2343,7 @@
       <c r="B19" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
@@ -2356,7 +2352,7 @@
       <c r="B20" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
@@ -2365,7 +2361,7 @@
       <c r="B21" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
@@ -2374,7 +2370,7 @@
       <c r="B22" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
@@ -2383,7 +2379,7 @@
       <c r="B23" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
@@ -2392,7 +2388,7 @@
       <c r="B24" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
@@ -2401,7 +2397,7 @@
       <c r="B25" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
@@ -2410,7 +2406,7 @@
       <c r="B26" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
@@ -2419,7 +2415,7 @@
       <c r="B27" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
@@ -2428,7 +2424,7 @@
       <c r="B28" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
@@ -2437,7 +2433,7 @@
       <c r="B29" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
@@ -2446,7 +2442,7 @@
       <c r="B30" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C30" s="11"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
@@ -2455,7 +2451,7 @@
       <c r="B31" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
@@ -2464,7 +2460,7 @@
       <c r="B32" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
@@ -2473,7 +2469,7 @@
       <c r="B33" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">

</xml_diff>

<commit_message>
Update mappings.xlsx with cleaned SupplierMappings
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -491,7 +491,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">By-Lo Oil Company  </t>
+          <t>By-Lo Oil Company</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">World Kinect          </t>
+          <t>World Kinect</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">

</xml_diff>

<commit_message>
✅ OPIS terminal injection and prompt updates
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -13,6 +13,7 @@
     <sheet name="SupplyLookupMappings" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="ProductMappings" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="TerminalMappings" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="OPIS_Terminal_Mappings" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="268">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -687,6 +688,147 @@
   </si>
   <si>
     <t xml:space="preserve">HARTFORD-IL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Terminal Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standardized Terminal Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Hartford - Phillips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Hartford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Wood River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houston - Magellan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasadena - Kinder Morgan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasadena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasadena - Vopak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas City - Magellan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Antonio - NuStar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Antonio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Hartford - Shell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houston - Kinder Morgan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Paso - Magellan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Paso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Chicago - Buckeye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Chicago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicago - CITGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicago - Kinder Morgan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Chicago - CITGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Hartford - Valero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasadena - Shell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des Moines - Magellan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des Moines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Louis, MO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wood River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Pasadena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Houston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cincinnati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OH Cincinnati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indianapolis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN Indianapolis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MN St. Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milwaukee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WI Milwaukee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN East Chicago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toledo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OH Toledo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WI Green Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IA Des Moines</t>
   </si>
 </sst>
 </file>
@@ -696,7 +838,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -724,6 +866,14 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -776,13 +926,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -979,8 +1141,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="A1:B32 C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -997,68 +1159,68 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1081,7 +1243,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1095,154 +1257,154 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1265,7 +1427,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1279,290 +1441,290 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1585,7 +1747,7 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1599,413 +1761,413 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="2" t="n">
         <v>870000000000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="2" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="2" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="2" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="2" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="2" t="n">
         <v>930000000000</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="2" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="2" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="2" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2028,7 +2190,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2045,272 +2207,272 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="2" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="2" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="2" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="2" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="2" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="2" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="2" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2323,4 +2485,284 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update: Refined OPIS prompt and extended terminal normalization mappings (added East St Louis)
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="270">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -829,6 +829,12 @@
   </si>
   <si>
     <t xml:space="preserve">IA Des Moines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East St. Louis, IL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL East St. Louis</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1148,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="A1:B32 C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1243,7 +1249,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1427,7 +1433,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1747,7 +1753,7 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2190,7 +2196,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2492,10 +2498,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2754,6 +2760,14 @@
       </c>
       <c r="B32" s="4" t="s">
         <v>267</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OPIS prompt and mappings.xlsx for improved terminal extraction
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="272">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -774,67 +774,73 @@
     <t xml:space="preserve">Des Moines</t>
   </si>
   <si>
+    <t xml:space="preserve">Wood River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Pasadena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Houston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cincinnati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OH Cincinnati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indianapolis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN Indianapolis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MN St. Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milwaukee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WI Milwaukee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN East Chicago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toledo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OH Toledo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WI Green Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IA Des Moines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East St. Louis, IL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL East St. Louis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST. LOUIS TERMINAL</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Louis, MO</t>
   </si>
   <si>
-    <t xml:space="preserve">Wood River</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX Pasadena</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX Houston</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cincinnati</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OH Cincinnati</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indianapolis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN Indianapolis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Paul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MN St. Paul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milwaukee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WI Milwaukee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN East Chicago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toledo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OH Toledo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WI Green Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IA Des Moines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East St. Louis, IL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL East St. Louis</t>
+    <t xml:space="preserve">FOB St. Louis</t>
   </si>
 </sst>
 </file>
@@ -2498,10 +2504,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2650,33 +2656,33 @@
         <v>248</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>168</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="B20" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>251</v>
@@ -2684,90 +2690,98 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>33</v>
+        <v>253</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="B32" s="4" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
         <v>267</v>
       </c>
+      <c r="B32" s="2" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="B33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>269</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update terminal mapping in mappings.xlsx with cleaned and capitalized values
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="260">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -81,6 +81,9 @@
     <t xml:space="preserve">mail.wallis.com</t>
   </si>
   <si>
+    <t xml:space="preserve">World Kinect Corporation</t>
+  </si>
+  <si>
     <t xml:space="preserve">WFS</t>
   </si>
   <si>
@@ -633,6 +636,21 @@
     <t xml:space="preserve">PSX Hartford PSX</t>
   </si>
   <si>
+    <t xml:space="preserve">SINCLAIR-HEP-KANSAS CITY-KS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kansas City KS Sinclair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Wood River - KMEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL, Cahokia, PSX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IA, Bettendorf, MG, Marathon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raw Terminal Name</t>
   </si>
   <si>
@@ -643,9 +661,6 @@
   </si>
   <si>
     <t xml:space="preserve">IL Hartford</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL Wood River - KMEP</t>
   </si>
   <si>
     <t xml:space="preserve">IL Wood River</t>
@@ -1127,10 +1142,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,6 +1230,17 @@
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1255,7 +1281,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -1263,130 +1289,130 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1417,234 +1443,234 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1695,410 +1721,410 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2129,8 +2155,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2147,413 +2173,445 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2603,274 +2661,274 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inject Volume Type mappings and prompt examples into parser and mappings
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -14,6 +14,7 @@
     <sheet name="ProductMappings" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="TerminalMappings" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="OPIS_Terminal_Mappings" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Volume_Type_Mappings" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="267">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -147,6 +148,9 @@
     <t xml:space="preserve">ExxonMobil</t>
   </si>
   <si>
+    <t xml:space="preserve">Mansfield</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prefix</t>
   </si>
   <si>
@@ -805,6 +809,24 @@
   </si>
   <si>
     <t xml:space="preserve">FOB St. Louis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kinder Morgan</t>
   </si>
 </sst>
 </file>
@@ -909,7 +931,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -947,6 +969,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1144,8 +1174,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="A1:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1262,7 +1292,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A1:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1413,6 +1443,14 @@
       </c>
       <c r="B18" s="2" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1436,22 +1474,22 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="A1:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
@@ -1459,7 +1497,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -1467,15 +1505,15 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
@@ -1483,34 +1521,34 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,12 +1556,12 @@
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>30</v>
@@ -1531,7 +1569,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>35</v>
@@ -1542,20 +1580,20 @@
         <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>21</v>
@@ -1563,7 +1601,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
@@ -1571,7 +1609,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>21</v>
@@ -1579,7 +1617,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
@@ -1587,7 +1625,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>21</v>
@@ -1595,7 +1633,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>29</v>
@@ -1603,15 +1641,15 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
@@ -1622,36 +1660,36 @@
         <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>20</v>
@@ -1659,7 +1697,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>35</v>
@@ -1667,7 +1705,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>26</v>
@@ -1701,7 +1739,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="topLeft" activeCell="A53" activeCellId="1" sqref="A1:D39 A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1721,410 +1759,410 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2156,7 +2194,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A1:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2173,445 +2211,445 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2654,185 +2692,185 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A1:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>217</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2840,95 +2878,672 @@
         <v>36</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>258</v>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="A1:D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="14.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="4" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Added supply override rule for By-Lo at Wood River KMEP to Grok prompt and mappings
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="298">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -151,6 +151,9 @@
     <t xml:space="preserve">Mansfield</t>
   </si>
   <si>
+    <t xml:space="preserve">Wood River - KMEP (By-Lo) </t>
+  </si>
+  <si>
     <t xml:space="preserve">Prefix</t>
   </si>
   <si>
@@ -251,6 +254,9 @@
   </si>
   <si>
     <t xml:space="preserve">Palmyra-Coffeyville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WR-BYLO </t>
   </si>
   <si>
     <t xml:space="preserve">ULSD</t>
@@ -1036,6 +1042,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1057,10 +1067,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1275,7 +1281,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="V5" activeCellId="0" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1392,7 +1398,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1551,6 +1557,14 @@
       </c>
       <c r="B19" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1573,23 +1587,23 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>20</v>
@@ -1597,7 +1611,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
@@ -1605,15 +1619,15 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>26</v>
@@ -1621,34 +1635,34 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,12 +1670,12 @@
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>30</v>
@@ -1669,7 +1683,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>35</v>
@@ -1680,20 +1694,20 @@
         <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>21</v>
@@ -1701,7 +1715,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>21</v>
@@ -1709,7 +1723,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>21</v>
@@ -1717,7 +1731,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>21</v>
@@ -1725,7 +1739,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>21</v>
@@ -1733,7 +1747,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>29</v>
@@ -1741,15 +1755,15 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>24</v>
@@ -1760,36 +1774,36 @@
         <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>20</v>
@@ -1797,18 +1811,26 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="A29" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1838,655 +1860,655 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="27.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="20.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="5" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="27.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="20.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="6" width="8.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>76</v>
+      <c r="A2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="10" t="n">
+        <v>890000000000</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10" t="n">
+        <v>910000000000</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="7" t="s">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="10" t="n">
+        <v>920000000000</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9" t="n">
-        <v>890000000000</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="n">
-        <v>910000000000</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="9" t="n">
-        <v>920000000000</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2536,445 +2558,445 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3024,178 +3046,178 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3203,95 +3225,95 @@
         <v>36</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3318,25 +3340,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="15.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="14.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="5" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="15.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="14.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="6" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,10 +3369,10 @@
         <v>20</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3361,10 +3383,10 @@
         <v>20</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,13 +3394,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3389,10 +3411,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3400,13 +3422,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,10 +3439,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3431,10 +3453,10 @@
         <v>30</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3445,10 +3467,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,13 +3478,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3473,10 +3495,10 @@
         <v>26</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3484,13 +3506,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3501,10 +3523,10 @@
         <v>24</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3512,13 +3534,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3529,10 +3551,10 @@
         <v>40</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3543,10 +3565,10 @@
         <v>35</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3557,10 +3579,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3571,10 +3593,10 @@
         <v>22</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,10 +3607,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3599,10 +3621,10 @@
         <v>21</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3613,10 +3635,10 @@
         <v>21</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3627,10 +3649,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3641,10 +3663,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3655,10 +3677,10 @@
         <v>26</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3666,13 +3688,13 @@
         <v>7</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3680,13 +3702,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3697,10 +3719,10 @@
         <v>35</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3711,10 +3733,10 @@
         <v>20</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3725,10 +3747,10 @@
         <v>21</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3739,10 +3761,10 @@
         <v>21</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3753,10 +3775,10 @@
         <v>21</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3764,13 +3786,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3778,13 +3800,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,13 +3814,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,13 +3828,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,13 +3842,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,13 +3856,13 @@
         <v>10</v>
       </c>
       <c r="B37" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D37" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,10 +3873,10 @@
         <v>21</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,10 +3887,10 @@
         <v>22</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update mappings.xlsx and supplier prompt for non-OPIS emails
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="298">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -1025,7 +1025,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1042,12 +1042,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1062,15 +1066,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1079,10 +1075,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1588,10 +1580,13 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.43"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1829,8 +1824,16 @@
       <c r="A30" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1866,424 +1869,424 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="27.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="20.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="6" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="27.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="7" width="8.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="9" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="9" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="7" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="7" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="9" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="9" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="9" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="9" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="9" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="7" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2291,7 +2294,7 @@
       <c r="A53" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="7" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2299,7 +2302,7 @@
       <c r="A54" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="7" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2307,7 +2310,7 @@
       <c r="A55" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="7" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2315,15 +2318,15 @@
       <c r="A56" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="7" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2331,7 +2334,7 @@
       <c r="A58" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="7" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2339,7 +2342,7 @@
       <c r="A59" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="7" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2347,7 +2350,7 @@
       <c r="A60" s="10" t="n">
         <v>890000000000</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="7" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2355,7 +2358,7 @@
       <c r="A61" s="10" t="n">
         <v>910000000000</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="7" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2363,7 +2366,7 @@
       <c r="A62" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="7" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2371,15 +2374,15 @@
       <c r="A63" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="7" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="7" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2387,7 +2390,7 @@
       <c r="A65" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="7" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2395,7 +2398,7 @@
       <c r="A66" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="7" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2403,7 +2406,7 @@
       <c r="A67" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2411,7 +2414,7 @@
       <c r="A68" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2419,7 +2422,7 @@
       <c r="A69" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="7" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2427,7 +2430,7 @@
       <c r="A70" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="7" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2435,7 +2438,7 @@
       <c r="A71" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="7" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2443,7 +2446,7 @@
       <c r="A72" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="7" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2451,7 +2454,7 @@
       <c r="A73" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="7" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2459,7 +2462,7 @@
       <c r="A74" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2467,7 +2470,7 @@
       <c r="A75" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2475,15 +2478,15 @@
       <c r="A76" s="10" t="n">
         <v>920000000000</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="7" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="7" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2491,7 +2494,7 @@
       <c r="A78" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="7" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2499,7 +2502,7 @@
       <c r="A79" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="7" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2507,7 +2510,7 @@
       <c r="A80" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="7" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2704,7 +2707,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="4" t="s">
         <v>196</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2712,7 +2715,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="4" t="s">
         <v>189</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2720,7 +2723,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2728,7 +2731,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="4" t="s">
         <v>186</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2736,7 +2739,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="4" t="s">
         <v>183</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2744,7 +2747,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="4" t="s">
         <v>200</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2752,7 +2755,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2760,7 +2763,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="4" t="s">
         <v>205</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2768,7 +2771,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="4" t="s">
         <v>207</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2776,7 +2779,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="4" t="s">
         <v>208</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2784,7 +2787,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="4" t="s">
         <v>209</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2792,7 +2795,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="4" t="s">
         <v>210</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2800,7 +2803,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="4" t="s">
         <v>211</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2808,7 +2811,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="4" t="s">
         <v>212</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2816,7 +2819,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="4" t="s">
         <v>214</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2824,7 +2827,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="4" t="s">
         <v>215</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2832,7 +2835,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="4" t="s">
         <v>216</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2840,7 +2843,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="4" t="s">
         <v>217</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2848,7 +2851,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="4" t="s">
         <v>218</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2856,7 +2859,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="4" t="s">
         <v>219</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2864,7 +2867,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="4" t="s">
         <v>220</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2872,7 +2875,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="4" t="s">
         <v>221</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2880,7 +2883,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="4" t="s">
         <v>223</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2888,7 +2891,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="4" t="s">
         <v>224</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2896,7 +2899,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="4" t="s">
         <v>226</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2904,7 +2907,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="4" t="s">
         <v>227</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2912,7 +2915,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2920,7 +2923,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="4" t="s">
         <v>230</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2928,7 +2931,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2936,7 +2939,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="4" t="s">
         <v>231</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2944,7 +2947,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="4" t="s">
         <v>232</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2952,7 +2955,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="4" t="s">
         <v>233</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2960,7 +2963,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="4" t="s">
         <v>234</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -3045,250 +3048,250 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="4" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="4" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="4" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="4" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="4" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="4" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="4" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="4" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="4" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="4" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="4" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="4" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="4" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="4" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="4" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="4" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="4" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="4" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="4" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="4" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="4" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="4" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="4" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="4" t="s">
         <v>286</v>
       </c>
     </row>
@@ -3340,556 +3343,556 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="15.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="14.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="14.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="7" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="10" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="10" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="10" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="10" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="10" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="10" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="10" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="10" t="s">
         <v>295</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ProductMappings for Wallis email variants
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="301">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -566,6 +566,15 @@
   </si>
   <si>
     <t xml:space="preserve">#2 Winter Dyed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">91E10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89E10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92E10</t>
   </si>
   <si>
     <t xml:space="preserve">Condition</t>
@@ -930,7 +939,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -966,6 +975,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1025,7 +1040,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1050,10 +1065,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1070,11 +1081,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1579,13 +1598,13 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,10 +1848,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1863,655 +1882,703 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="27.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="7" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="27.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="20.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="6" width="8.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="6" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="6" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="6" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="10" t="n">
+      <c r="A60" s="6" t="n">
         <v>890000000000</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="n">
+      <c r="A61" s="6" t="n">
         <v>910000000000</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="6" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="6" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="6" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="6" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="6" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="10" t="n">
+      <c r="A76" s="6" t="n">
         <v>920000000000</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="6" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="6" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="6" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2561,141 +2628,141 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2703,231 +2770,231 @@
         <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2935,71 +3002,71 @@
         <v>75</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3048,179 +3115,179 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>241</v>
+      <c r="A1" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,95 +3295,95 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -3343,557 +3410,557 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="14.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="7" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="15.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="14.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="6" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>294</v>
+      <c r="C1" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>295</v>
+      <c r="C2" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="D20" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="C25" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="C29" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="C30" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="C35" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="C36" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>295</v>
+      <c r="C39" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update terminal mappings to handle @ ColumbiaMG outliers
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="304">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -755,6 +755,15 @@
   </si>
   <si>
     <t xml:space="preserve">IA, Bettendorf, MG, Marathon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTP ENRGY~ @ ColumbiaMG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROWMARK @ ColumbiaMG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">*@ ColumbiaMG</t>
   </si>
   <si>
     <t xml:space="preserve">Raw Terminal Name</t>
@@ -1040,7 +1049,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1087,6 +1096,10 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1882,7 +1895,7 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
     </sheetView>
   </sheetViews>
@@ -2610,13 +2623,13 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.35"/>
   </cols>
   <sheetData>
@@ -3067,6 +3080,30 @@
       </c>
       <c r="B55" s="1" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3115,19 +3152,19 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>244</v>
+      <c r="A1" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3135,159 +3172,159 @@
         <v>240</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3295,95 +3332,95 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -3418,17 +3455,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>297</v>
+      <c r="C1" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,7 +3479,7 @@
         <v>202</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,7 +3493,7 @@
         <v>190</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3470,7 +3507,7 @@
         <v>185</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3484,7 +3521,7 @@
         <v>204</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3498,7 +3535,7 @@
         <v>216</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3512,7 +3549,7 @@
         <v>216</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3526,7 +3563,7 @@
         <v>216</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,7 +3577,7 @@
         <v>216</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3554,7 +3591,7 @@
         <v>216</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3568,7 +3605,7 @@
         <v>216</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3582,7 +3619,7 @@
         <v>216</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3596,7 +3633,7 @@
         <v>216</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,7 +3647,7 @@
         <v>216</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3624,7 +3661,7 @@
         <v>216</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3638,7 +3675,7 @@
         <v>225</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3652,7 +3689,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3666,7 +3703,7 @@
         <v>196</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3680,7 +3717,7 @@
         <v>228</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,7 +3731,7 @@
         <v>187</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,7 +3745,7 @@
         <v>231</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3722,7 +3759,7 @@
         <v>204</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3736,7 +3773,7 @@
         <v>207</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3750,7 +3787,7 @@
         <v>205</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3764,7 +3801,7 @@
         <v>205</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3778,7 +3815,7 @@
         <v>205</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,7 +3829,7 @@
         <v>225</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,7 +3843,7 @@
         <v>190</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,7 +3857,7 @@
         <v>187</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,7 +3871,7 @@
         <v>204</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3848,7 +3885,7 @@
         <v>207</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3862,7 +3899,7 @@
         <v>194</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3876,7 +3913,7 @@
         <v>209</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3890,7 +3927,7 @@
         <v>209</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3904,7 +3941,7 @@
         <v>239</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3918,7 +3955,7 @@
         <v>209</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,13 +3963,13 @@
         <v>10</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>190</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3946,7 +3983,7 @@
         <v>187</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3960,7 +3997,7 @@
         <v>194</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update mappings.xlsx: add Scott City and Champaign terminal and product mappings
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="306">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -625,6 +625,9 @@
     <t xml:space="preserve">Scott City MO Enterprise</t>
   </si>
   <si>
+    <t xml:space="preserve">DKTS/Scott City EN</t>
+  </si>
+  <si>
     <t xml:space="preserve">KM-WOOD RIVER</t>
   </si>
   <si>
@@ -764,6 +767,9 @@
   </si>
   <si>
     <t xml:space="preserve">*@ ColumbiaMG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPC/Champaign MPC</t>
   </si>
   <si>
     <t xml:space="preserve">Raw Terminal Name</t>
@@ -948,7 +954,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -984,12 +990,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1049,7 +1049,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1090,23 +1090,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1895,8 +1887,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2579,19 +2571,27 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="B85" s="10" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="10" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2623,7 +2623,7 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
     </sheetView>
   </sheetViews>
@@ -2711,151 +2711,151 @@
         <v>199</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>199</v>
-      </c>
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2863,7 +2863,7 @@
         <v>211</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2871,7 +2871,7 @@
         <v>212</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2879,7 +2879,7 @@
         <v>213</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2887,7 +2887,7 @@
         <v>214</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2895,15 +2895,15 @@
         <v>215</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2911,7 +2911,7 @@
         <v>218</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2919,7 +2919,7 @@
         <v>219</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2927,7 +2927,7 @@
         <v>220</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2935,7 +2935,7 @@
         <v>221</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2943,7 +2943,7 @@
         <v>222</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2951,7 +2951,7 @@
         <v>223</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2959,15 +2959,15 @@
         <v>224</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2975,15 +2975,15 @@
         <v>227</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2991,15 +2991,15 @@
         <v>230</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3007,23 +3007,23 @@
         <v>233</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>75</v>
+        <v>234</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>234</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3031,7 +3031,7 @@
         <v>235</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3039,7 +3039,7 @@
         <v>236</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3047,23 +3047,23 @@
         <v>237</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="4" t="s">
         <v>238</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3071,7 +3071,7 @@
         <v>241</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3079,34 +3079,49 @@
         <v>242</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="4" t="s">
         <v>244</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="4" t="s">
         <v>245</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3152,179 +3167,179 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>247</v>
+      <c r="A1" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3332,95 +3347,95 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -3455,17 +3470,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>300</v>
+      <c r="C1" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3476,10 +3491,10 @@
         <v>20</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3493,7 +3508,7 @@
         <v>190</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3507,7 +3522,7 @@
         <v>185</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3518,10 +3533,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3532,10 +3547,10 @@
         <v>59</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,10 +3561,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3560,10 +3575,10 @@
         <v>30</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3574,10 +3589,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3588,10 +3603,10 @@
         <v>69</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3602,10 +3617,10 @@
         <v>26</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3616,10 +3631,10 @@
         <v>71</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3630,10 +3645,10 @@
         <v>24</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3644,10 +3659,10 @@
         <v>52</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3658,10 +3673,10 @@
         <v>40</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,10 +3687,10 @@
         <v>35</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3689,7 +3704,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3703,7 +3718,7 @@
         <v>196</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,10 +3729,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3731,7 +3746,7 @@
         <v>187</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3742,10 +3757,10 @@
         <v>21</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3756,10 +3771,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3770,10 +3785,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,10 +3799,10 @@
         <v>26</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,10 +3813,10 @@
         <v>52</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3812,10 +3827,10 @@
         <v>59</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3826,10 +3841,10 @@
         <v>35</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,7 +3858,7 @@
         <v>190</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3857,7 +3872,7 @@
         <v>187</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3868,10 +3883,10 @@
         <v>21</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3882,10 +3897,10 @@
         <v>21</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3899,7 +3914,7 @@
         <v>194</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3910,10 +3925,10 @@
         <v>50</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,10 +3939,10 @@
         <v>52</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3938,10 +3953,10 @@
         <v>69</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3952,10 +3967,10 @@
         <v>71</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3963,13 +3978,13 @@
         <v>10</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>190</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3983,7 +3998,7 @@
         <v>187</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3997,7 +4012,7 @@
         <v>194</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Add BP/Wood River terminal and RFG product mappings for Grok Mini support
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="306">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -1887,8 +1887,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2592,6 +2592,14 @@
       </c>
       <c r="B87" s="6" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2623,8 +2631,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update mappings.xlsx: normalize 'R' product variants and improve deduplication support
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="308">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -628,6 +628,9 @@
     <t xml:space="preserve">DKTS/Scott City EN</t>
   </si>
   <si>
+    <t xml:space="preserve">DKTS/Scott City EN – Net</t>
+  </si>
+  <si>
     <t xml:space="preserve">KM-WOOD RIVER</t>
   </si>
   <si>
@@ -770,6 +773,9 @@
   </si>
   <si>
     <t xml:space="preserve">MPC/Champaign MPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPC/Champaign MPC Gross</t>
   </si>
   <si>
     <t xml:space="preserve">Raw Terminal Name</t>
@@ -1049,7 +1055,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1091,6 +1097,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1887,7 +1897,7 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
     </sheetView>
   </sheetViews>
@@ -2631,8 +2641,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2723,155 +2733,155 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="11" t="s">
         <v>200</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="B20" s="1" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2879,7 +2889,7 @@
         <v>212</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2887,7 +2897,7 @@
         <v>213</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2895,7 +2905,7 @@
         <v>214</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2903,7 +2913,7 @@
         <v>215</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2911,15 +2921,15 @@
         <v>216</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2927,7 +2937,7 @@
         <v>219</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2935,7 +2945,7 @@
         <v>220</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2943,7 +2953,7 @@
         <v>221</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2951,7 +2961,7 @@
         <v>222</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2959,7 +2969,7 @@
         <v>223</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2967,7 +2977,7 @@
         <v>224</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2975,15 +2985,15 @@
         <v>225</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2991,15 +3001,15 @@
         <v>228</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>229</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3007,15 +3017,15 @@
         <v>231</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3023,23 +3033,23 @@
         <v>234</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>75</v>
+        <v>235</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>235</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3047,7 +3057,7 @@
         <v>236</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3055,7 +3065,7 @@
         <v>237</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3063,23 +3073,23 @@
         <v>238</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="4" t="s">
         <v>239</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3087,7 +3097,7 @@
         <v>242</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3095,15 +3105,15 @@
         <v>243</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3111,26 +3121,41 @@
         <v>245</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="4" t="s">
         <v>246</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3168,186 +3193,186 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>249</v>
+      <c r="A1" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3355,95 +3380,95 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -3478,17 +3503,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>302</v>
+      <c r="C1" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3499,10 +3524,10 @@
         <v>20</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3516,7 +3541,7 @@
         <v>190</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3530,7 +3555,7 @@
         <v>185</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3541,10 +3566,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3555,10 +3580,10 @@
         <v>59</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,10 +3594,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3583,10 +3608,10 @@
         <v>30</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3597,10 +3622,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3611,10 +3636,10 @@
         <v>69</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3625,10 +3650,10 @@
         <v>26</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3639,10 +3664,10 @@
         <v>71</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3653,10 +3678,10 @@
         <v>24</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3667,10 +3692,10 @@
         <v>52</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,10 +3706,10 @@
         <v>40</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3695,10 +3720,10 @@
         <v>35</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3712,7 +3737,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3726,7 +3751,7 @@
         <v>196</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3737,10 +3762,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3754,7 +3779,7 @@
         <v>187</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3765,10 +3790,10 @@
         <v>21</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3779,10 +3804,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3793,10 +3818,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3807,10 +3832,10 @@
         <v>26</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3821,10 +3846,10 @@
         <v>52</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3835,10 +3860,10 @@
         <v>59</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3849,10 +3874,10 @@
         <v>35</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3866,7 +3891,7 @@
         <v>190</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3880,7 +3905,7 @@
         <v>187</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,10 +3916,10 @@
         <v>21</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,10 +3930,10 @@
         <v>21</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3922,7 +3947,7 @@
         <v>194</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3933,10 +3958,10 @@
         <v>50</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3947,10 +3972,10 @@
         <v>52</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3961,10 +3986,10 @@
         <v>69</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3975,10 +4000,10 @@
         <v>71</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3986,13 +4011,13 @@
         <v>10</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>190</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4006,7 +4031,7 @@
         <v>187</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4020,7 +4045,7 @@
         <v>194</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update mappings.xlsx with latest supplier/product/terminal updates
</commit_message>
<xml_diff>
--- a/mappings.xlsx
+++ b/mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SupplierMappings" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="314">
   <si>
     <t xml:space="preserve">Raw Value</t>
   </si>
@@ -154,6 +154,12 @@
     <t xml:space="preserve">Wood River - KMEP (By-Lo) </t>
   </si>
   <si>
+    <t xml:space="preserve">BioU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BioUrja</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prefix</t>
   </si>
   <si>
@@ -778,6 +784,15 @@
     <t xml:space="preserve">MPC/Champaign MPC Gross</t>
   </si>
   <si>
+    <t xml:space="preserve">BioU/STL KM South</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint Louis MO Kinder Morgan South</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STL KM South</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raw Terminal Name</t>
   </si>
   <si>
@@ -950,6 +965,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kinder Morgan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BioU </t>
   </si>
 </sst>
 </file>
@@ -960,7 +978,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -996,6 +1014,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1055,7 +1079,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1073,6 +1097,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1100,15 +1128,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1424,7 +1452,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1591,6 +1619,14 @@
       </c>
       <c r="B20" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1614,7 +1650,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1624,15 +1660,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>20</v>
@@ -1640,7 +1676,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
@@ -1648,15 +1684,15 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>26</v>
@@ -1664,34 +1700,34 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,12 +1735,12 @@
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>30</v>
@@ -1712,7 +1748,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>35</v>
@@ -1723,20 +1759,20 @@
         <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>21</v>
@@ -1744,7 +1780,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>21</v>
@@ -1752,7 +1788,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>21</v>
@@ -1760,7 +1796,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>21</v>
@@ -1768,7 +1804,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>21</v>
@@ -1776,7 +1812,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>29</v>
@@ -1784,15 +1820,15 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>24</v>
@@ -1803,36 +1839,36 @@
         <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>20</v>
@@ -1840,23 +1876,23 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>20</v>
@@ -1868,6 +1904,14 @@
       </c>
       <c r="B31" s="4" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1903,713 +1947,713 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="27.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="20.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="6" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="27.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="7" width="8.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>78</v>
+      <c r="A2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="n">
+        <v>890000000000</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7" t="n">
+        <v>910000000000</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="7" t="n">
+        <v>920000000000</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="B82" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="8" t="s">
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6" t="n">
-        <v>890000000000</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="6" t="n">
-        <v>910000000000</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="6" t="n">
-        <v>920000000000</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2641,8 +2685,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2659,501 +2703,517 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11" t="s">
-        <v>249</v>
+      <c r="A62" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3193,186 +3253,186 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>251</v>
+      <c r="A1" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3380,95 +3440,95 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -3487,565 +3547,579 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="15.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="14.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="14.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="7" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>304</v>
+      <c r="A1" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>305</v>
+      <c r="C2" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>306</v>
+      <c r="C3" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="C32" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="C38" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>305</v>
+      <c r="B40" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>